<commit_message>
CBIT Listo, queda aplicar los cambios a periferia
</commit_message>
<xml_diff>
--- a/CONTACTOS FACTURACION Y CARTERA.xlsx
+++ b/CONTACTOS FACTURACION Y CARTERA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\Periferia IT Group\Digital Prophets Team\RPA\estadoCuentas\RPA_EstadodeCuentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B617D24-BE13-49EE-BAF0-A84EBB47DAA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338F9ED7-3441-4399-A4EF-D13DD9F81896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{08BB3D2A-86CF-4B09-A994-13C08E1CCA5A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{08BB3D2A-86CF-4B09-A994-13C08E1CCA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="CBIT " sheetId="1" r:id="rId1"/>
@@ -2253,29 +2253,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2292,13 +2280,43 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2307,24 +2325,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2734,11 +2734,11 @@
   </sheetPr>
   <dimension ref="A1:AC1007"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2807,55 +2807,55 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="127" t="s">
+      <c r="D6" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="127" t="s">
+      <c r="E6" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="127" t="s">
+      <c r="F6" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="117" t="s">
+      <c r="G6" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="132" t="s">
+      <c r="H6" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="117" t="s">
+      <c r="I6" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="119" t="s">
+      <c r="J6" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="119" t="s">
+      <c r="K6" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="119" t="s">
+      <c r="L6" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="121" t="s">
+      <c r="M6" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="123" t="s">
+      <c r="N6" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="119" t="s">
+      <c r="O6" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="119" t="s">
+      <c r="P6" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="121" t="s">
+      <c r="Q6" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="123" t="s">
+      <c r="R6" s="119" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2870,13 +2870,13 @@
       <c r="I7" s="118"/>
       <c r="J7" s="118"/>
       <c r="K7" s="118"/>
-      <c r="L7" s="120"/>
-      <c r="M7" s="122"/>
-      <c r="N7" s="124"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="131"/>
+      <c r="N7" s="132"/>
       <c r="O7" s="118"/>
-      <c r="P7" s="120"/>
+      <c r="P7" s="130"/>
       <c r="Q7" s="118"/>
-      <c r="R7" s="125"/>
+      <c r="R7" s="120"/>
     </row>
     <row r="8" spans="1:18" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="77" t="s">
@@ -2964,7 +2964,7 @@
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="130" t="s">
+      <c r="B10" s="126" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -3001,7 +3001,7 @@
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B11" s="131"/>
+      <c r="B11" s="127"/>
       <c r="C11" s="61" t="s">
         <v>42</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="A12" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="124" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="61" t="s">
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="128"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="5" t="s">
         <v>69</v>
       </c>
@@ -3151,7 +3151,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="128"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="61" t="s">
         <v>81</v>
       </c>
@@ -3198,7 +3198,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="128"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="61" t="s">
         <v>92</v>
       </c>
@@ -3247,7 +3247,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="128"/>
+      <c r="B16" s="124"/>
       <c r="C16" s="5" t="s">
         <v>96</v>
       </c>
@@ -3286,7 +3286,7 @@
       <c r="R16" s="18"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="128"/>
+      <c r="B17" s="124"/>
       <c r="C17" s="5" t="s">
         <v>102</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="R17" s="18"/>
     </row>
     <row r="18" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="128"/>
+      <c r="B18" s="124"/>
       <c r="C18" s="61" t="s">
         <v>495</v>
       </c>
@@ -3365,7 +3365,7 @@
       </c>
     </row>
     <row r="19" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="125" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -3414,7 +3414,7 @@
       </c>
     </row>
     <row r="20" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B20" s="129"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="40" t="s">
         <v>124</v>
       </c>
@@ -3447,7 +3447,7 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B21" s="129"/>
+      <c r="B21" s="125"/>
       <c r="C21" s="40" t="s">
         <v>131</v>
       </c>
@@ -3482,7 +3482,7 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B22" s="129"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="40" t="s">
         <v>138</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:29" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B23" s="129"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="40" t="s">
         <v>144</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:29" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="124" t="s">
         <v>149</v>
       </c>
       <c r="C24" s="61" t="s">
@@ -3605,7 +3605,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" s="23" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="128"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="61" t="s">
         <v>158</v>
       </c>
@@ -3703,7 +3703,7 @@
       <c r="AC26" s="9"/>
     </row>
     <row r="27" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="126" t="s">
+      <c r="B27" s="122" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="61" t="s">
@@ -3746,7 +3746,7 @@
       </c>
     </row>
     <row r="28" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="126"/>
+      <c r="B28" s="122"/>
       <c r="C28" s="61" t="s">
         <v>186</v>
       </c>
@@ -11556,6 +11556,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="J6:J7"/>
@@ -11572,12 +11578,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M24" r:id="rId1" xr:uid="{F19620FB-438A-4AD7-8B24-7ABCF787291C}"/>
@@ -11632,7 +11632,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:R989"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -11708,62 +11708,62 @@
       <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="135" t="s">
+      <c r="B6" s="141" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="137" t="s">
+      <c r="C6" s="143" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="138" t="s">
+      <c r="D6" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="139" t="s">
+      <c r="E6" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="139" t="s">
+      <c r="F6" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="133" t="s">
+      <c r="G6" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="133" t="s">
+      <c r="H6" s="137" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="133" t="s">
+      <c r="I6" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="140" t="s">
+      <c r="J6" s="133" t="s">
         <v>190</v>
       </c>
-      <c r="K6" s="140" t="s">
+      <c r="K6" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="143" t="s">
+      <c r="L6" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="140" t="s">
+      <c r="M6" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="139" t="s">
+      <c r="N6" s="138" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="140" t="s">
+      <c r="O6" s="133" t="s">
         <v>191</v>
       </c>
-      <c r="P6" s="143" t="s">
+      <c r="P6" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="140" t="s">
+      <c r="Q6" s="133" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="141" t="s">
+      <c r="R6" s="135" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="136"/>
+      <c r="B7" s="142"/>
       <c r="C7" s="134"/>
-      <c r="D7" s="136"/>
+      <c r="D7" s="142"/>
       <c r="E7" s="134"/>
       <c r="F7" s="134"/>
       <c r="G7" s="134"/>
@@ -11771,13 +11771,13 @@
       <c r="I7" s="134"/>
       <c r="J7" s="134"/>
       <c r="K7" s="134"/>
-      <c r="L7" s="144"/>
+      <c r="L7" s="140"/>
       <c r="M7" s="134"/>
       <c r="N7" s="134"/>
       <c r="O7" s="134"/>
-      <c r="P7" s="144"/>
+      <c r="P7" s="140"/>
       <c r="Q7" s="134"/>
-      <c r="R7" s="142"/>
+      <c r="R7" s="136"/>
     </row>
     <row r="8" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -20934,6 +20934,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
@@ -20945,12 +20951,6 @@
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="P6:P7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M8" r:id="rId1" xr:uid="{16FF0051-4D26-43D9-AB14-A91026794FA3}"/>
@@ -21036,6 +21036,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000C8E1A23AEA2D14D9F691681F0E710B9" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fe88c6cfb13cb3c476d9df96f1dd7198">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fbfa516-ef3c-4fb1-8499-0c478f39e0d9" xmlns:ns3="84954463-2ec1-410a-8a4d-bda7d1bc08f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd586fcd70b8c8e818bc3b921b53f5f5" ns2:_="" ns3:_="">
     <xsd:import namespace="0fbfa516-ef3c-4fb1-8499-0c478f39e0d9"/>
@@ -21246,15 +21255,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -21262,6 +21262,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BDFCC4-8940-4AED-A665-06A70F630966}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB4F2EBC-5E00-4D84-A86E-34B42AC8FC67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21280,14 +21288,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BDFCC4-8940-4AED-A665-06A70F630966}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169E4E83-4648-4187-B0AA-E35AC5867923}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
CBIT Listo, Periferia Listo :)
</commit_message>
<xml_diff>
--- a/CONTACTOS FACTURACION Y CARTERA.xlsx
+++ b/CONTACTOS FACTURACION Y CARTERA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\Documents\Periferia IT Group\Digital Prophets Team\RPA\estadoCuentas\RPA_EstadodeCuentas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338F9ED7-3441-4399-A4EF-D13DD9F81896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848C3BE7-2783-4F9A-A98A-B4CD08B6CFD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{08BB3D2A-86CF-4B09-A994-13C08E1CCA5A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{08BB3D2A-86CF-4B09-A994-13C08E1CCA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="CBIT " sheetId="1" r:id="rId1"/>
@@ -2253,17 +2253,29 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2280,43 +2292,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2325,6 +2307,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2734,11 +2734,11 @@
   </sheetPr>
   <dimension ref="A1:AC1007"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="7" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2807,55 +2807,55 @@
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="123" t="s">
+      <c r="D6" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="123" t="s">
+      <c r="E6" s="127" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="123" t="s">
+      <c r="F6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="128" t="s">
+      <c r="G6" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="129" t="s">
+      <c r="H6" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="128" t="s">
+      <c r="I6" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="121" t="s">
+      <c r="J6" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="121" t="s">
+      <c r="K6" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="121" t="s">
+      <c r="L6" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="117" t="s">
+      <c r="M6" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="119" t="s">
+      <c r="N6" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="121" t="s">
+      <c r="O6" s="119" t="s">
         <v>12</v>
       </c>
-      <c r="P6" s="121" t="s">
+      <c r="P6" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="117" t="s">
+      <c r="Q6" s="121" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="119" t="s">
+      <c r="R6" s="123" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2870,13 +2870,13 @@
       <c r="I7" s="118"/>
       <c r="J7" s="118"/>
       <c r="K7" s="118"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="131"/>
-      <c r="N7" s="132"/>
+      <c r="L7" s="120"/>
+      <c r="M7" s="122"/>
+      <c r="N7" s="124"/>
       <c r="O7" s="118"/>
-      <c r="P7" s="130"/>
+      <c r="P7" s="120"/>
       <c r="Q7" s="118"/>
-      <c r="R7" s="120"/>
+      <c r="R7" s="125"/>
     </row>
     <row r="8" spans="1:18" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="77" t="s">
@@ -2964,7 +2964,7 @@
       <c r="R9" s="5"/>
     </row>
     <row r="10" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="126" t="s">
+      <c r="B10" s="130" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -3001,7 +3001,7 @@
       <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:18" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B11" s="127"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="61" t="s">
         <v>42</v>
       </c>
@@ -3051,7 +3051,7 @@
       <c r="A12" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="124" t="s">
+      <c r="B12" s="128" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="61" t="s">
@@ -3104,7 +3104,7 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="124"/>
+      <c r="B13" s="128"/>
       <c r="C13" s="5" t="s">
         <v>69</v>
       </c>
@@ -3151,7 +3151,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="124"/>
+      <c r="B14" s="128"/>
       <c r="C14" s="61" t="s">
         <v>81</v>
       </c>
@@ -3198,7 +3198,7 @@
       </c>
     </row>
     <row r="15" spans="1:18" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="124"/>
+      <c r="B15" s="128"/>
       <c r="C15" s="61" t="s">
         <v>92</v>
       </c>
@@ -3247,7 +3247,7 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="124"/>
+      <c r="B16" s="128"/>
       <c r="C16" s="5" t="s">
         <v>96</v>
       </c>
@@ -3286,7 +3286,7 @@
       <c r="R16" s="18"/>
     </row>
     <row r="17" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="124"/>
+      <c r="B17" s="128"/>
       <c r="C17" s="5" t="s">
         <v>102</v>
       </c>
@@ -3316,7 +3316,7 @@
       <c r="R17" s="18"/>
     </row>
     <row r="18" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="124"/>
+      <c r="B18" s="128"/>
       <c r="C18" s="61" t="s">
         <v>495</v>
       </c>
@@ -3365,7 +3365,7 @@
       </c>
     </row>
     <row r="19" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="129" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -3414,7 +3414,7 @@
       </c>
     </row>
     <row r="20" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B20" s="125"/>
+      <c r="B20" s="129"/>
       <c r="C20" s="40" t="s">
         <v>124</v>
       </c>
@@ -3447,7 +3447,7 @@
       <c r="R20" s="5"/>
     </row>
     <row r="21" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B21" s="125"/>
+      <c r="B21" s="129"/>
       <c r="C21" s="40" t="s">
         <v>131</v>
       </c>
@@ -3482,7 +3482,7 @@
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="B22" s="125"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="40" t="s">
         <v>138</v>
       </c>
@@ -3517,7 +3517,7 @@
       <c r="R22" s="5"/>
     </row>
     <row r="23" spans="1:29" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B23" s="125"/>
+      <c r="B23" s="129"/>
       <c r="C23" s="40" t="s">
         <v>144</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="R23" s="5"/>
     </row>
     <row r="24" spans="1:29" s="23" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B24" s="124" t="s">
+      <c r="B24" s="128" t="s">
         <v>149</v>
       </c>
       <c r="C24" s="61" t="s">
@@ -3605,7 +3605,7 @@
       </c>
     </row>
     <row r="25" spans="1:29" s="23" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="124"/>
+      <c r="B25" s="128"/>
       <c r="C25" s="61" t="s">
         <v>158</v>
       </c>
@@ -3703,7 +3703,7 @@
       <c r="AC26" s="9"/>
     </row>
     <row r="27" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="122" t="s">
+      <c r="B27" s="126" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="61" t="s">
@@ -3746,7 +3746,7 @@
       </c>
     </row>
     <row r="28" spans="1:29" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="122"/>
+      <c r="B28" s="126"/>
       <c r="C28" s="61" t="s">
         <v>186</v>
       </c>
@@ -11556,12 +11556,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
     <mergeCell ref="J6:J7"/>
@@ -11578,6 +11572,12 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M24" r:id="rId1" xr:uid="{F19620FB-438A-4AD7-8B24-7ABCF787291C}"/>
@@ -11632,7 +11632,7 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:R989"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="7" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -11708,62 +11708,62 @@
       <c r="I5" s="28"/>
     </row>
     <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="141" t="s">
+      <c r="B6" s="135" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="143" t="s">
+      <c r="C6" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="139" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="138" t="s">
+      <c r="F6" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="137" t="s">
+      <c r="G6" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="137" t="s">
+      <c r="H6" s="133" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="137" t="s">
+      <c r="I6" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="133" t="s">
+      <c r="J6" s="140" t="s">
         <v>190</v>
       </c>
-      <c r="K6" s="133" t="s">
+      <c r="K6" s="140" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="139" t="s">
+      <c r="L6" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="133" t="s">
+      <c r="M6" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="138" t="s">
+      <c r="N6" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="133" t="s">
+      <c r="O6" s="140" t="s">
         <v>191</v>
       </c>
-      <c r="P6" s="139" t="s">
+      <c r="P6" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="133" t="s">
+      <c r="Q6" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="135" t="s">
+      <c r="R6" s="141" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="142"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="134"/>
-      <c r="D7" s="142"/>
+      <c r="D7" s="136"/>
       <c r="E7" s="134"/>
       <c r="F7" s="134"/>
       <c r="G7" s="134"/>
@@ -11771,13 +11771,13 @@
       <c r="I7" s="134"/>
       <c r="J7" s="134"/>
       <c r="K7" s="134"/>
-      <c r="L7" s="140"/>
+      <c r="L7" s="144"/>
       <c r="M7" s="134"/>
       <c r="N7" s="134"/>
       <c r="O7" s="134"/>
-      <c r="P7" s="140"/>
+      <c r="P7" s="144"/>
       <c r="Q7" s="134"/>
-      <c r="R7" s="136"/>
+      <c r="R7" s="142"/>
     </row>
     <row r="8" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
@@ -20934,12 +20934,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="Q6:Q7"/>
     <mergeCell ref="R6:R7"/>
@@ -20951,6 +20945,12 @@
     <mergeCell ref="N6:N7"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="P6:P7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="M8" r:id="rId1" xr:uid="{16FF0051-4D26-43D9-AB14-A91026794FA3}"/>
@@ -21036,15 +21036,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000C8E1A23AEA2D14D9F691681F0E710B9" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fe88c6cfb13cb3c476d9df96f1dd7198">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fbfa516-ef3c-4fb1-8499-0c478f39e0d9" xmlns:ns3="84954463-2ec1-410a-8a4d-bda7d1bc08f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd586fcd70b8c8e818bc3b921b53f5f5" ns2:_="" ns3:_="">
     <xsd:import namespace="0fbfa516-ef3c-4fb1-8499-0c478f39e0d9"/>
@@ -21255,6 +21246,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -21262,14 +21262,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BDFCC4-8940-4AED-A665-06A70F630966}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB4F2EBC-5E00-4D84-A86E-34B42AC8FC67}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21288,6 +21280,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7BDFCC4-8940-4AED-A665-06A70F630966}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{169E4E83-4648-4187-B0AA-E35AC5867923}">
   <ds:schemaRefs>

</xml_diff>